<commit_message>
Version 09-25 - Large changes to qoq and ifoCAST evaluation
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/1_GDP_series/absolute_combined_GDP.xlsx
+++ b/0_0_Data/2_Processed_Data/1_GDP_series/absolute_combined_GDP.xlsx
@@ -369,13 +369,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ER222"/>
+  <dimension ref="A1:ES223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:148">
+    <row r="1" spans="1:149">
       <c r="B1" s="1">
         <v>32508</v>
       </c>
@@ -817,8 +817,11 @@
       <c r="ER1" s="1">
         <v>45800</v>
       </c>
+      <c r="ES1" s="1">
+        <v>45891</v>
+      </c>
     </row>
-    <row r="2" spans="1:148">
+    <row r="2" spans="1:149">
       <c r="A2" s="1">
         <v>25569</v>
       </c>
@@ -1263,8 +1266,11 @@
       <c r="ER2">
         <v>38.49</v>
       </c>
+      <c r="ES2">
+        <v>38.50631393048884</v>
+      </c>
     </row>
-    <row r="3" spans="1:148">
+    <row r="3" spans="1:149">
       <c r="A3" s="1">
         <v>25659</v>
       </c>
@@ -1709,8 +1715,11 @@
       <c r="ER3">
         <v>40.01</v>
       </c>
+      <c r="ES3">
+        <v>40.02695818027691</v>
+      </c>
     </row>
-    <row r="4" spans="1:148">
+    <row r="4" spans="1:149">
       <c r="A4" s="1">
         <v>25750</v>
       </c>
@@ -2155,8 +2164,11 @@
       <c r="ER4">
         <v>40.76</v>
       </c>
+      <c r="ES4">
+        <v>40.7772760666855</v>
+      </c>
     </row>
-    <row r="5" spans="1:148">
+    <row r="5" spans="1:149">
       <c r="A5" s="1">
         <v>25842</v>
       </c>
@@ -2601,8 +2613,11 @@
       <c r="ER5">
         <v>41.11</v>
       </c>
+      <c r="ES5">
+        <v>41.12742441367618</v>
+      </c>
     </row>
-    <row r="6" spans="1:148">
+    <row r="6" spans="1:149">
       <c r="A6" s="1">
         <v>25934</v>
       </c>
@@ -3047,8 +3062,11 @@
       <c r="ER6">
         <v>40.31</v>
       </c>
+      <c r="ES6">
+        <v>40.32708533484035</v>
+      </c>
     </row>
-    <row r="7" spans="1:148">
+    <row r="7" spans="1:149">
       <c r="A7" s="1">
         <v>26024</v>
       </c>
@@ -3493,8 +3511,11 @@
       <c r="ER7">
         <v>41.17</v>
       </c>
+      <c r="ES7">
+        <v>41.18744984458887</v>
+      </c>
     </row>
-    <row r="8" spans="1:148">
+    <row r="8" spans="1:149">
       <c r="A8" s="1">
         <v>26115</v>
       </c>
@@ -3939,8 +3960,11 @@
       <c r="ER8">
         <v>41.87</v>
       </c>
+      <c r="ES8">
+        <v>41.88774653857022</v>
+      </c>
     </row>
-    <row r="9" spans="1:148">
+    <row r="9" spans="1:149">
       <c r="A9" s="1">
         <v>26207</v>
       </c>
@@ -4385,8 +4409,11 @@
       <c r="ER9">
         <v>41.83</v>
       </c>
+      <c r="ES9">
+        <v>41.84772958462842</v>
+      </c>
     </row>
-    <row r="10" spans="1:148">
+    <row r="10" spans="1:149">
       <c r="A10" s="1">
         <v>26299</v>
       </c>
@@ -4831,8 +4858,11 @@
       <c r="ER10">
         <v>41.87</v>
       </c>
+      <c r="ES10">
+        <v>41.88774653857022</v>
+      </c>
     </row>
-    <row r="11" spans="1:148">
+    <row r="11" spans="1:149">
       <c r="A11" s="1">
         <v>26390</v>
       </c>
@@ -5277,8 +5307,11 @@
       <c r="ER11">
         <v>42.56</v>
       </c>
+      <c r="ES11">
+        <v>42.57803899406613</v>
+      </c>
     </row>
-    <row r="12" spans="1:148">
+    <row r="12" spans="1:149">
       <c r="A12" s="1">
         <v>26481</v>
       </c>
@@ -5723,8 +5756,11 @@
       <c r="ER12">
         <v>43.55</v>
       </c>
+      <c r="ES12">
+        <v>43.56845860412546</v>
+      </c>
     </row>
-    <row r="13" spans="1:148">
+    <row r="13" spans="1:149">
       <c r="A13" s="1">
         <v>26573</v>
       </c>
@@ -6169,8 +6205,11 @@
       <c r="ER13">
         <v>44.22</v>
       </c>
+      <c r="ES13">
+        <v>44.23874258265047</v>
+      </c>
     </row>
-    <row r="14" spans="1:148">
+    <row r="14" spans="1:149">
       <c r="A14" s="1">
         <v>26665</v>
       </c>
@@ -6615,8 +6654,11 @@
       <c r="ER14">
         <v>44.86</v>
       </c>
+      <c r="ES14">
+        <v>44.87901384571913</v>
+      </c>
     </row>
-    <row r="15" spans="1:148">
+    <row r="15" spans="1:149">
       <c r="A15" s="1">
         <v>26755</v>
       </c>
@@ -7061,8 +7103,11 @@
       <c r="ER15">
         <v>45.17</v>
       </c>
+      <c r="ES15">
+        <v>45.18914523876802</v>
+      </c>
     </row>
-    <row r="16" spans="1:148">
+    <row r="16" spans="1:149">
       <c r="A16" s="1">
         <v>26846</v>
       </c>
@@ -7507,8 +7552,11 @@
       <c r="ER16">
         <v>45.33</v>
       </c>
+      <c r="ES16">
+        <v>45.34921305453518</v>
+      </c>
     </row>
-    <row r="17" spans="1:148">
+    <row r="17" spans="1:149">
       <c r="A17" s="1">
         <v>26938</v>
       </c>
@@ -7953,8 +8001,11 @@
       <c r="ER17">
         <v>45.43</v>
       </c>
+      <c r="ES17">
+        <v>45.44925543938966</v>
+      </c>
     </row>
-    <row r="18" spans="1:148">
+    <row r="18" spans="1:149">
       <c r="A18" s="1">
         <v>27030</v>
       </c>
@@ -8399,8 +8450,11 @@
       <c r="ER18">
         <v>45.81</v>
       </c>
+      <c r="ES18">
+        <v>45.82941650183668</v>
+      </c>
     </row>
-    <row r="19" spans="1:148">
+    <row r="19" spans="1:149">
       <c r="A19" s="1">
         <v>27120</v>
       </c>
@@ -8845,8 +8899,11 @@
       <c r="ER19">
         <v>45.77</v>
       </c>
+      <c r="ES19">
+        <v>45.78939954789489</v>
+      </c>
     </row>
-    <row r="20" spans="1:148">
+    <row r="20" spans="1:149">
       <c r="A20" s="1">
         <v>27211</v>
       </c>
@@ -9291,8 +9348,11 @@
       <c r="ER20">
         <v>45.78</v>
       </c>
+      <c r="ES20">
+        <v>45.79940378638034</v>
+      </c>
     </row>
-    <row r="21" spans="1:148">
+    <row r="21" spans="1:149">
       <c r="A21" s="1">
         <v>27303</v>
       </c>
@@ -9737,8 +9797,11 @@
       <c r="ER21">
         <v>45.21</v>
       </c>
+      <c r="ES21">
+        <v>45.22916219270981</v>
+      </c>
     </row>
-    <row r="22" spans="1:148">
+    <row r="22" spans="1:149">
       <c r="A22" s="1">
         <v>27395</v>
       </c>
@@ -10183,8 +10246,11 @@
       <c r="ER22">
         <v>44.95</v>
       </c>
+      <c r="ES22">
+        <v>44.96905199208817</v>
+      </c>
     </row>
-    <row r="23" spans="1:148">
+    <row r="23" spans="1:149">
       <c r="A23" s="1">
         <v>27485</v>
       </c>
@@ -10629,8 +10695,11 @@
       <c r="ER23">
         <v>44.72</v>
       </c>
+      <c r="ES23">
+        <v>44.73895450692286</v>
+      </c>
     </row>
-    <row r="24" spans="1:148">
+    <row r="24" spans="1:149">
       <c r="A24" s="1">
         <v>27576</v>
       </c>
@@ -11075,8 +11144,11 @@
       <c r="ER24">
         <v>45.21</v>
       </c>
+      <c r="ES24">
+        <v>45.22916219270981</v>
+      </c>
     </row>
-    <row r="25" spans="1:148">
+    <row r="25" spans="1:149">
       <c r="A25" s="1">
         <v>27668</v>
       </c>
@@ -11521,8 +11593,11 @@
       <c r="ER25">
         <v>46.1</v>
       </c>
+      <c r="ES25">
+        <v>46.11953941791467</v>
+      </c>
     </row>
-    <row r="26" spans="1:148">
+    <row r="26" spans="1:149">
       <c r="A26" s="1">
         <v>27760</v>
       </c>
@@ -11967,8 +12042,11 @@
       <c r="ER26">
         <v>46.5</v>
       </c>
+      <c r="ES26">
+        <v>46.51970895733258</v>
+      </c>
     </row>
-    <row r="27" spans="1:148">
+    <row r="27" spans="1:149">
       <c r="A27" s="1">
         <v>27851</v>
       </c>
@@ -12413,8 +12491,11 @@
       <c r="ER27">
         <v>47.2</v>
       </c>
+      <c r="ES27">
+        <v>47.22000565131393</v>
+      </c>
     </row>
-    <row r="28" spans="1:148">
+    <row r="28" spans="1:149">
       <c r="A28" s="1">
         <v>27942</v>
       </c>
@@ -12859,8 +12940,11 @@
       <c r="ER28">
         <v>47.21</v>
       </c>
+      <c r="ES28">
+        <v>47.23000988979938</v>
+      </c>
     </row>
-    <row r="29" spans="1:148">
+    <row r="29" spans="1:149">
       <c r="A29" s="1">
         <v>28034</v>
       </c>
@@ -13305,8 +13389,11 @@
       <c r="ER29">
         <v>48.09</v>
       </c>
+      <c r="ES29">
+        <v>48.1103828765188</v>
+      </c>
     </row>
-    <row r="30" spans="1:148">
+    <row r="30" spans="1:149">
       <c r="A30" s="1">
         <v>28126</v>
       </c>
@@ -13751,8 +13838,11 @@
       <c r="ER30">
         <v>48.51</v>
       </c>
+      <c r="ES30">
+        <v>48.5305608929076</v>
+      </c>
     </row>
-    <row r="31" spans="1:148">
+    <row r="31" spans="1:149">
       <c r="A31" s="1">
         <v>28216</v>
       </c>
@@ -14197,8 +14287,11 @@
       <c r="ER31">
         <v>48.78</v>
       </c>
+      <c r="ES31">
+        <v>48.8006753320147</v>
+      </c>
     </row>
-    <row r="32" spans="1:148">
+    <row r="32" spans="1:149">
       <c r="A32" s="1">
         <v>28307</v>
       </c>
@@ -14643,8 +14736,11 @@
       <c r="ER32">
         <v>48.76</v>
       </c>
+      <c r="ES32">
+        <v>48.7806668550438</v>
+      </c>
     </row>
-    <row r="33" spans="1:148">
+    <row r="33" spans="1:149">
       <c r="A33" s="1">
         <v>28399</v>
       </c>
@@ -15089,8 +15185,11 @@
       <c r="ER33">
         <v>49.6</v>
       </c>
+      <c r="ES33">
+        <v>49.62102288782143</v>
+      </c>
     </row>
-    <row r="34" spans="1:148">
+    <row r="34" spans="1:149">
       <c r="A34" s="1">
         <v>28491</v>
       </c>
@@ -15535,8 +15634,11 @@
       <c r="ER34">
         <v>49.8</v>
       </c>
+      <c r="ES34">
+        <v>49.82110765753038</v>
+      </c>
     </row>
-    <row r="35" spans="1:148">
+    <row r="35" spans="1:149">
       <c r="A35" s="1">
         <v>28581</v>
       </c>
@@ -15981,8 +16083,11 @@
       <c r="ER35">
         <v>50.01</v>
       </c>
+      <c r="ES35">
+        <v>50.03119666572479</v>
+      </c>
     </row>
-    <row r="36" spans="1:148">
+    <row r="36" spans="1:149">
       <c r="A36" s="1">
         <v>28672</v>
       </c>
@@ -16427,8 +16532,11 @@
       <c r="ER36">
         <v>50.66</v>
       </c>
+      <c r="ES36">
+        <v>50.68147216727889</v>
+      </c>
     </row>
-    <row r="37" spans="1:148">
+    <row r="37" spans="1:149">
       <c r="A37" s="1">
         <v>28764</v>
       </c>
@@ -16873,8 +16981,11 @@
       <c r="ER37">
         <v>51.25</v>
       </c>
+      <c r="ES37">
+        <v>51.27172223792032</v>
+      </c>
     </row>
-    <row r="38" spans="1:148">
+    <row r="38" spans="1:149">
       <c r="A38" s="1">
         <v>28856</v>
       </c>
@@ -17319,8 +17430,11 @@
       <c r="ER38">
         <v>51.32</v>
       </c>
+      <c r="ES38">
+        <v>51.34175190731845</v>
+      </c>
     </row>
-    <row r="39" spans="1:148">
+    <row r="39" spans="1:149">
       <c r="A39" s="1">
         <v>28946</v>
       </c>
@@ -17765,8 +17879,11 @@
       <c r="ER39">
         <v>52.91</v>
       </c>
+      <c r="ES39">
+        <v>52.93242582650466</v>
+      </c>
     </row>
-    <row r="40" spans="1:148">
+    <row r="40" spans="1:149">
       <c r="A40" s="1">
         <v>29037</v>
       </c>
@@ -18211,8 +18328,11 @@
       <c r="ER40">
         <v>52.91</v>
       </c>
+      <c r="ES40">
+        <v>52.93242582650466</v>
+      </c>
     </row>
-    <row r="41" spans="1:148">
+    <row r="41" spans="1:149">
       <c r="A41" s="1">
         <v>29129</v>
       </c>
@@ -18657,8 +18777,11 @@
       <c r="ER41">
         <v>53.24</v>
       </c>
+      <c r="ES41">
+        <v>53.26256569652445</v>
+      </c>
     </row>
-    <row r="42" spans="1:148">
+    <row r="42" spans="1:149">
       <c r="A42" s="1">
         <v>29221</v>
       </c>
@@ -19103,8 +19226,11 @@
       <c r="ER42">
         <v>53.66</v>
       </c>
+      <c r="ES42">
+        <v>53.68274371291325</v>
+      </c>
     </row>
-    <row r="43" spans="1:148">
+    <row r="43" spans="1:149">
       <c r="A43" s="1">
         <v>29312</v>
       </c>
@@ -19549,8 +19675,11 @@
       <c r="ER43">
         <v>53.31</v>
       </c>
+      <c r="ES43">
+        <v>53.33259536592258</v>
+      </c>
     </row>
-    <row r="44" spans="1:148">
+    <row r="44" spans="1:149">
       <c r="A44" s="1">
         <v>29403</v>
       </c>
@@ -19995,8 +20124,11 @@
       <c r="ER44">
         <v>53.09</v>
       </c>
+      <c r="ES44">
+        <v>53.11250211924273</v>
+      </c>
     </row>
-    <row r="45" spans="1:148">
+    <row r="45" spans="1:149">
       <c r="A45" s="1">
         <v>29495</v>
       </c>
@@ -20441,8 +20573,11 @@
       <c r="ER45">
         <v>53.02</v>
       </c>
+      <c r="ES45">
+        <v>53.0424724498446</v>
+      </c>
     </row>
-    <row r="46" spans="1:148">
+    <row r="46" spans="1:149">
       <c r="A46" s="1">
         <v>29587</v>
       </c>
@@ -20887,8 +21022,11 @@
       <c r="ER46">
         <v>53.66</v>
       </c>
+      <c r="ES46">
+        <v>53.68274371291325</v>
+      </c>
     </row>
-    <row r="47" spans="1:148">
+    <row r="47" spans="1:149">
       <c r="A47" s="1">
         <v>29677</v>
       </c>
@@ -21333,8 +21471,11 @@
       <c r="ER47">
         <v>53.52</v>
       </c>
+      <c r="ES47">
+        <v>53.54268437411699</v>
+      </c>
     </row>
-    <row r="48" spans="1:148">
+    <row r="48" spans="1:149">
       <c r="A48" s="1">
         <v>29768</v>
       </c>
@@ -21779,8 +21920,11 @@
       <c r="ER48">
         <v>53.67</v>
       </c>
+      <c r="ES48">
+        <v>53.69274795139871</v>
+      </c>
     </row>
-    <row r="49" spans="1:148">
+    <row r="49" spans="1:149">
       <c r="A49" s="1">
         <v>29860</v>
       </c>
@@ -22225,8 +22369,11 @@
       <c r="ER49">
         <v>53.61</v>
       </c>
+      <c r="ES49">
+        <v>53.63272252048601</v>
+      </c>
     </row>
-    <row r="50" spans="1:148">
+    <row r="50" spans="1:149">
       <c r="A50" s="1">
         <v>29952</v>
       </c>
@@ -22671,8 +22818,11 @@
       <c r="ER50">
         <v>53.83</v>
       </c>
+      <c r="ES50">
+        <v>53.85281576716586</v>
+      </c>
     </row>
-    <row r="51" spans="1:148">
+    <row r="51" spans="1:149">
       <c r="A51" s="1">
         <v>30042</v>
       </c>
@@ -23117,8 +23267,11 @@
       <c r="ER51">
         <v>53.49</v>
       </c>
+      <c r="ES51">
+        <v>53.51267165866064</v>
+      </c>
     </row>
-    <row r="52" spans="1:148">
+    <row r="52" spans="1:149">
       <c r="A52" s="1">
         <v>30133</v>
       </c>
@@ -23563,8 +23716,11 @@
       <c r="ER52">
         <v>52.98</v>
       </c>
+      <c r="ES52">
+        <v>53.00245549590279</v>
+      </c>
     </row>
-    <row r="53" spans="1:148">
+    <row r="53" spans="1:149">
       <c r="A53" s="1">
         <v>30225</v>
       </c>
@@ -24009,8 +24165,11 @@
       <c r="ER53">
         <v>53.09</v>
       </c>
+      <c r="ES53">
+        <v>53.11250211924273</v>
+      </c>
     </row>
-    <row r="54" spans="1:148">
+    <row r="54" spans="1:149">
       <c r="A54" s="1">
         <v>30317</v>
       </c>
@@ -24455,8 +24614,11 @@
       <c r="ER54">
         <v>53.58</v>
       </c>
+      <c r="ES54">
+        <v>53.60270980502967</v>
+      </c>
     </row>
-    <row r="55" spans="1:148">
+    <row r="55" spans="1:149">
       <c r="A55" s="1">
         <v>30407</v>
       </c>
@@ -24901,8 +25063,11 @@
       <c r="ER55">
         <v>54.15</v>
       </c>
+      <c r="ES55">
+        <v>54.1729513987002</v>
+      </c>
     </row>
-    <row r="56" spans="1:148">
+    <row r="56" spans="1:149">
       <c r="A56" s="1">
         <v>30498</v>
       </c>
@@ -25347,8 +25512,11 @@
       <c r="ER56">
         <v>54.02</v>
       </c>
+      <c r="ES56">
+        <v>54.04289629838938</v>
+      </c>
     </row>
-    <row r="57" spans="1:148">
+    <row r="57" spans="1:149">
       <c r="A57" s="1">
         <v>30590</v>
       </c>
@@ -25793,8 +25961,11 @@
       <c r="ER57">
         <v>54.77</v>
       </c>
+      <c r="ES57">
+        <v>54.79321418479798</v>
+      </c>
     </row>
-    <row r="58" spans="1:148">
+    <row r="58" spans="1:149">
       <c r="A58" s="1">
         <v>30682</v>
       </c>
@@ -26239,8 +26410,11 @@
       <c r="ER58">
         <v>55.49</v>
       </c>
+      <c r="ES58">
+        <v>55.51351935575022</v>
+      </c>
     </row>
-    <row r="59" spans="1:148">
+    <row r="59" spans="1:149">
       <c r="A59" s="1">
         <v>30773</v>
       </c>
@@ -26685,8 +26859,11 @@
       <c r="ER59">
         <v>54.62</v>
       </c>
+      <c r="ES59">
+        <v>54.64315060751625</v>
+      </c>
     </row>
-    <row r="60" spans="1:148">
+    <row r="60" spans="1:149">
       <c r="A60" s="1">
         <v>30864</v>
       </c>
@@ -27131,8 +27308,11 @@
       <c r="ER60">
         <v>56.11</v>
       </c>
+      <c r="ES60">
+        <v>56.13378214184798</v>
+      </c>
     </row>
-    <row r="61" spans="1:148">
+    <row r="61" spans="1:149">
       <c r="A61" s="1">
         <v>30956</v>
       </c>
@@ -27577,8 +27757,11 @@
       <c r="ER61">
         <v>56.58</v>
       </c>
+      <c r="ES61">
+        <v>56.60398135066403</v>
+      </c>
     </row>
-    <row r="62" spans="1:148">
+    <row r="62" spans="1:149">
       <c r="A62" s="1">
         <v>31048</v>
       </c>
@@ -28023,8 +28206,11 @@
       <c r="ER62">
         <v>56.28</v>
       </c>
+      <c r="ES62">
+        <v>56.30385419610059</v>
+      </c>
     </row>
-    <row r="63" spans="1:148">
+    <row r="63" spans="1:149">
       <c r="A63" s="1">
         <v>31138</v>
       </c>
@@ -28469,8 +28655,11 @@
       <c r="ER63">
         <v>56.83</v>
       </c>
+      <c r="ES63">
+        <v>56.85408731280022</v>
+      </c>
     </row>
-    <row r="64" spans="1:148">
+    <row r="64" spans="1:149">
       <c r="A64" s="1">
         <v>31229</v>
       </c>
@@ -28915,8 +29104,11 @@
       <c r="ER64">
         <v>57.57</v>
       </c>
+      <c r="ES64">
+        <v>57.59440096072337</v>
+      </c>
     </row>
-    <row r="65" spans="1:148">
+    <row r="65" spans="1:149">
       <c r="A65" s="1">
         <v>31321</v>
       </c>
@@ -29361,8 +29553,11 @@
       <c r="ER65">
         <v>57.92</v>
       </c>
+      <c r="ES65">
+        <v>57.94454930771405</v>
+      </c>
     </row>
-    <row r="66" spans="1:148">
+    <row r="66" spans="1:149">
       <c r="A66" s="1">
         <v>31413</v>
       </c>
@@ -29807,8 +30002,11 @@
       <c r="ER66">
         <v>57.59</v>
       </c>
+      <c r="ES66">
+        <v>57.61440943769427</v>
+      </c>
     </row>
-    <row r="67" spans="1:148">
+    <row r="67" spans="1:149">
       <c r="A67" s="1">
         <v>31503</v>
       </c>
@@ -30253,8 +30451,11 @@
       <c r="ER67">
         <v>58.26</v>
       </c>
+      <c r="ES67">
+        <v>58.28469341621927</v>
+      </c>
     </row>
-    <row r="68" spans="1:148">
+    <row r="68" spans="1:149">
       <c r="A68" s="1">
         <v>31594</v>
       </c>
@@ -30699,8 +30900,11 @@
       <c r="ER68">
         <v>58.69</v>
       </c>
+      <c r="ES68">
+        <v>58.71487567109353</v>
+      </c>
     </row>
-    <row r="69" spans="1:148">
+    <row r="69" spans="1:149">
       <c r="A69" s="1">
         <v>31686</v>
       </c>
@@ -31145,8 +31349,11 @@
       <c r="ER69">
         <v>59.27</v>
       </c>
+      <c r="ES69">
+        <v>59.29512150324951</v>
+      </c>
     </row>
-    <row r="70" spans="1:148">
+    <row r="70" spans="1:149">
       <c r="A70" s="1">
         <v>31778</v>
       </c>
@@ -31591,8 +31798,11 @@
       <c r="ER70">
         <v>57.78</v>
       </c>
+      <c r="ES70">
+        <v>57.80448996891778</v>
+      </c>
     </row>
-    <row r="71" spans="1:148">
+    <row r="71" spans="1:149">
       <c r="A71" s="1">
         <v>31868</v>
       </c>
@@ -32037,8 +32247,11 @@
       <c r="ER71">
         <v>59.08</v>
       </c>
+      <c r="ES71">
+        <v>59.105040972026</v>
+      </c>
     </row>
-    <row r="72" spans="1:148">
+    <row r="72" spans="1:149">
       <c r="A72" s="1">
         <v>31959</v>
       </c>
@@ -32483,8 +32696,11 @@
       <c r="ER72">
         <v>59.5</v>
       </c>
+      <c r="ES72">
+        <v>59.52521898841481</v>
+      </c>
     </row>
-    <row r="73" spans="1:148">
+    <row r="73" spans="1:149">
       <c r="A73" s="1">
         <v>32051</v>
       </c>
@@ -32929,8 +33145,11 @@
       <c r="ER73">
         <v>60.44</v>
       </c>
+      <c r="ES73">
+        <v>60.46561740604691</v>
+      </c>
     </row>
-    <row r="74" spans="1:148">
+    <row r="74" spans="1:149">
       <c r="A74" s="1">
         <v>32143</v>
       </c>
@@ -33375,8 +33594,11 @@
       <c r="ER74">
         <v>59.9</v>
       </c>
+      <c r="ES74">
+        <v>59.92538852783272</v>
+      </c>
     </row>
-    <row r="75" spans="1:148">
+    <row r="75" spans="1:149">
       <c r="A75" s="1">
         <v>32234</v>
       </c>
@@ -33821,8 +34043,11 @@
       <c r="ER75">
         <v>60.99</v>
       </c>
+      <c r="ES75">
+        <v>61.01585052274655</v>
+      </c>
     </row>
-    <row r="76" spans="1:148">
+    <row r="76" spans="1:149">
       <c r="A76" s="1">
         <v>32325</v>
       </c>
@@ -34267,8 +34492,11 @@
       <c r="ER76">
         <v>61.66</v>
       </c>
+      <c r="ES76">
+        <v>61.68613450127155</v>
+      </c>
     </row>
-    <row r="77" spans="1:148">
+    <row r="77" spans="1:149">
       <c r="A77" s="1">
         <v>32417</v>
       </c>
@@ -34710,8 +34938,11 @@
       <c r="ER77">
         <v>62.4</v>
       </c>
+      <c r="ES77">
+        <v>62.42644814919469</v>
+      </c>
     </row>
-    <row r="78" spans="1:148">
+    <row r="78" spans="1:149">
       <c r="A78" s="1">
         <v>32509</v>
       </c>
@@ -35150,8 +35381,11 @@
       <c r="ER78">
         <v>63.04</v>
       </c>
+      <c r="ES78">
+        <v>63.06671941226335</v>
+      </c>
     </row>
-    <row r="79" spans="1:148">
+    <row r="79" spans="1:149">
       <c r="A79" s="1">
         <v>32599</v>
       </c>
@@ -35587,8 +35821,11 @@
       <c r="ER79">
         <v>63.3</v>
       </c>
+      <c r="ES79">
+        <v>63.326829612885</v>
+      </c>
     </row>
-    <row r="80" spans="1:148">
+    <row r="80" spans="1:149">
       <c r="A80" s="1">
         <v>32690</v>
       </c>
@@ -36021,8 +36258,11 @@
       <c r="ER80">
         <v>63.87</v>
       </c>
+      <c r="ES80">
+        <v>63.89707120655552</v>
+      </c>
     </row>
-    <row r="81" spans="1:148">
+    <row r="81" spans="1:149">
       <c r="A81" s="1">
         <v>32782</v>
       </c>
@@ -36452,8 +36692,11 @@
       <c r="ER81">
         <v>64.62</v>
       </c>
+      <c r="ES81">
+        <v>64.64738909296412</v>
+      </c>
     </row>
-    <row r="82" spans="1:148">
+    <row r="82" spans="1:149">
       <c r="A82" s="1">
         <v>32874</v>
       </c>
@@ -36880,8 +37123,11 @@
       <c r="ER82">
         <v>65.95999999999999</v>
       </c>
+      <c r="ES82">
+        <v>65.98795705001413</v>
+      </c>
     </row>
-    <row r="83" spans="1:148">
+    <row r="83" spans="1:149">
       <c r="A83" s="1">
         <v>32964</v>
       </c>
@@ -37305,8 +37551,11 @@
       <c r="ER83">
         <v>66.28</v>
       </c>
+      <c r="ES83">
+        <v>66.30809268154846</v>
+      </c>
     </row>
-    <row r="84" spans="1:148">
+    <row r="84" spans="1:149">
       <c r="A84" s="1">
         <v>33055</v>
       </c>
@@ -37727,8 +37976,11 @@
       <c r="ER84">
         <v>67.68000000000001</v>
       </c>
+      <c r="ES84">
+        <v>67.70868606951117</v>
+      </c>
     </row>
-    <row r="85" spans="1:148">
+    <row r="85" spans="1:149">
       <c r="A85" s="1">
         <v>33147</v>
       </c>
@@ -38146,8 +38398,11 @@
       <c r="ER85">
         <v>68.88</v>
       </c>
+      <c r="ES85">
+        <v>68.90919468776491</v>
+      </c>
     </row>
-    <row r="86" spans="1:148">
+    <row r="86" spans="1:149">
       <c r="A86" s="1">
         <v>33239</v>
       </c>
@@ -38562,8 +38817,11 @@
       <c r="ER86">
         <v>70.78</v>
       </c>
+      <c r="ES86">
+        <v>70.81</v>
+      </c>
     </row>
-    <row r="87" spans="1:148">
+    <row r="87" spans="1:149">
       <c r="A87" s="1">
         <v>33329</v>
       </c>
@@ -38975,8 +39233,11 @@
       <c r="ER87">
         <v>70.47</v>
       </c>
+      <c r="ES87">
+        <v>70.47</v>
+      </c>
     </row>
-    <row r="88" spans="1:148">
+    <row r="88" spans="1:149">
       <c r="A88" s="1">
         <v>33420</v>
       </c>
@@ -39385,8 +39646,11 @@
       <c r="ER88">
         <v>70.34</v>
       </c>
+      <c r="ES88">
+        <v>70.36</v>
+      </c>
     </row>
-    <row r="89" spans="1:148">
+    <row r="89" spans="1:149">
       <c r="A89" s="1">
         <v>33512</v>
       </c>
@@ -39792,8 +40056,11 @@
       <c r="ER89">
         <v>71.33</v>
       </c>
+      <c r="ES89">
+        <v>71.37</v>
+      </c>
     </row>
-    <row r="90" spans="1:148">
+    <row r="90" spans="1:149">
       <c r="A90" s="1">
         <v>33604</v>
       </c>
@@ -40196,8 +40463,11 @@
       <c r="ER90">
         <v>72.34</v>
       </c>
+      <c r="ES90">
+        <v>72.34999999999999</v>
+      </c>
     </row>
-    <row r="91" spans="1:148">
+    <row r="91" spans="1:149">
       <c r="A91" s="1">
         <v>33695</v>
       </c>
@@ -40597,8 +40867,11 @@
       <c r="ER91">
         <v>71.90000000000001</v>
       </c>
+      <c r="ES91">
+        <v>71.90000000000001</v>
+      </c>
     </row>
-    <row r="92" spans="1:148">
+    <row r="92" spans="1:149">
       <c r="A92" s="1">
         <v>33786</v>
       </c>
@@ -40995,8 +41268,11 @@
       <c r="ER92">
         <v>71.70999999999999</v>
       </c>
+      <c r="ES92">
+        <v>71.73</v>
+      </c>
     </row>
-    <row r="93" spans="1:148">
+    <row r="93" spans="1:149">
       <c r="A93" s="1">
         <v>33878</v>
       </c>
@@ -41390,8 +41666,11 @@
       <c r="ER93">
         <v>71.5</v>
       </c>
+      <c r="ES93">
+        <v>71.53</v>
+      </c>
     </row>
-    <row r="94" spans="1:148">
+    <row r="94" spans="1:149">
       <c r="A94" s="1">
         <v>33970</v>
       </c>
@@ -41782,8 +42061,11 @@
       <c r="ER94">
         <v>70.94</v>
       </c>
+      <c r="ES94">
+        <v>70.95999999999999</v>
+      </c>
     </row>
-    <row r="95" spans="1:148">
+    <row r="95" spans="1:149">
       <c r="A95" s="1">
         <v>34060</v>
       </c>
@@ -42171,8 +42453,11 @@
       <c r="ER95">
         <v>70.97</v>
       </c>
+      <c r="ES95">
+        <v>70.97</v>
+      </c>
     </row>
-    <row r="96" spans="1:148">
+    <row r="96" spans="1:149">
       <c r="A96" s="1">
         <v>34151</v>
       </c>
@@ -42557,8 +42842,11 @@
       <c r="ER96">
         <v>71.37</v>
       </c>
+      <c r="ES96">
+        <v>71.39</v>
+      </c>
     </row>
-    <row r="97" spans="1:148">
+    <row r="97" spans="1:149">
       <c r="A97" s="1">
         <v>34243</v>
       </c>
@@ -42940,8 +43228,11 @@
       <c r="ER97">
         <v>71.31999999999999</v>
       </c>
+      <c r="ES97">
+        <v>71.33</v>
+      </c>
     </row>
-    <row r="98" spans="1:148">
+    <row r="98" spans="1:149">
       <c r="A98" s="1">
         <v>34335</v>
       </c>
@@ -43320,8 +43611,11 @@
       <c r="ER98">
         <v>72.31</v>
       </c>
+      <c r="ES98">
+        <v>72.34</v>
+      </c>
     </row>
-    <row r="99" spans="1:148">
+    <row r="99" spans="1:149">
       <c r="A99" s="1">
         <v>34425</v>
       </c>
@@ -43697,8 +43991,11 @@
       <c r="ER99">
         <v>72.73</v>
       </c>
+      <c r="ES99">
+        <v>72.73999999999999</v>
+      </c>
     </row>
-    <row r="100" spans="1:148">
+    <row r="100" spans="1:149">
       <c r="A100" s="1">
         <v>34516</v>
       </c>
@@ -44071,8 +44368,11 @@
       <c r="ER100">
         <v>73.15000000000001</v>
       </c>
+      <c r="ES100">
+        <v>73.17</v>
+      </c>
     </row>
-    <row r="101" spans="1:148">
+    <row r="101" spans="1:149">
       <c r="A101" s="1">
         <v>34608</v>
       </c>
@@ -44442,8 +44742,11 @@
       <c r="ER101">
         <v>73.97</v>
       </c>
+      <c r="ES101">
+        <v>73.98</v>
+      </c>
     </row>
-    <row r="102" spans="1:148">
+    <row r="102" spans="1:149">
       <c r="A102" s="1">
         <v>34700</v>
       </c>
@@ -44810,8 +45113,11 @@
       <c r="ER102">
         <v>73.67</v>
       </c>
+      <c r="ES102">
+        <v>73.69</v>
+      </c>
     </row>
-    <row r="103" spans="1:148">
+    <row r="103" spans="1:149">
       <c r="A103" s="1">
         <v>34790</v>
       </c>
@@ -45175,8 +45481,11 @@
       <c r="ER103">
         <v>74.27</v>
       </c>
+      <c r="ES103">
+        <v>74.28</v>
+      </c>
     </row>
-    <row r="104" spans="1:148">
+    <row r="104" spans="1:149">
       <c r="A104" s="1">
         <v>34881</v>
       </c>
@@ -45537,8 +45846,11 @@
       <c r="ER104">
         <v>74.40000000000001</v>
       </c>
+      <c r="ES104">
+        <v>74.43000000000001</v>
+      </c>
     </row>
-    <row r="105" spans="1:148">
+    <row r="105" spans="1:149">
       <c r="A105" s="1">
         <v>34973</v>
       </c>
@@ -45896,8 +46208,11 @@
       <c r="ER105">
         <v>74.43000000000001</v>
       </c>
+      <c r="ES105">
+        <v>74.45999999999999</v>
+      </c>
     </row>
-    <row r="106" spans="1:148">
+    <row r="106" spans="1:149">
       <c r="A106" s="1">
         <v>35065</v>
       </c>
@@ -46252,8 +46567,11 @@
       <c r="ER106">
         <v>73.91</v>
       </c>
+      <c r="ES106">
+        <v>73.93000000000001</v>
+      </c>
     </row>
-    <row r="107" spans="1:148">
+    <row r="107" spans="1:149">
       <c r="A107" s="1">
         <v>35156</v>
       </c>
@@ -46605,8 +46923,11 @@
       <c r="ER107">
         <v>74.94</v>
       </c>
+      <c r="ES107">
+        <v>74.94</v>
+      </c>
     </row>
-    <row r="108" spans="1:148">
+    <row r="108" spans="1:149">
       <c r="A108" s="1">
         <v>35247</v>
       </c>
@@ -46955,8 +47276,11 @@
       <c r="ER108">
         <v>75.2</v>
       </c>
+      <c r="ES108">
+        <v>75.23</v>
+      </c>
     </row>
-    <row r="109" spans="1:148">
+    <row r="109" spans="1:149">
       <c r="A109" s="1">
         <v>35339</v>
       </c>
@@ -47302,8 +47626,11 @@
       <c r="ER109">
         <v>75.88</v>
       </c>
+      <c r="ES109">
+        <v>75.92</v>
+      </c>
     </row>
-    <row r="110" spans="1:148">
+    <row r="110" spans="1:149">
       <c r="A110" s="1">
         <v>35431</v>
       </c>
@@ -47646,8 +47973,11 @@
       <c r="ER110">
         <v>75.52</v>
       </c>
+      <c r="ES110">
+        <v>75.53</v>
+      </c>
     </row>
-    <row r="111" spans="1:148">
+    <row r="111" spans="1:149">
       <c r="A111" s="1">
         <v>35521</v>
       </c>
@@ -47987,8 +48317,11 @@
       <c r="ER111">
         <v>76.37</v>
       </c>
+      <c r="ES111">
+        <v>76.37</v>
+      </c>
     </row>
-    <row r="112" spans="1:148">
+    <row r="112" spans="1:149">
       <c r="A112" s="1">
         <v>35612</v>
       </c>
@@ -48325,8 +48658,11 @@
       <c r="ER112">
         <v>76.64</v>
       </c>
+      <c r="ES112">
+        <v>76.67</v>
+      </c>
     </row>
-    <row r="113" spans="1:148">
+    <row r="113" spans="1:149">
       <c r="A113" s="1">
         <v>35704</v>
       </c>
@@ -48660,8 +48996,11 @@
       <c r="ER113">
         <v>77.20999999999999</v>
       </c>
+      <c r="ES113">
+        <v>77.23999999999999</v>
+      </c>
     </row>
-    <row r="114" spans="1:148">
+    <row r="114" spans="1:149">
       <c r="A114" s="1">
         <v>35796</v>
       </c>
@@ -48992,8 +49331,11 @@
       <c r="ER114">
         <v>77.97</v>
       </c>
+      <c r="ES114">
+        <v>77.98</v>
+      </c>
     </row>
-    <row r="115" spans="1:148">
+    <row r="115" spans="1:149">
       <c r="A115" s="1">
         <v>35886</v>
       </c>
@@ -49321,8 +49663,11 @@
       <c r="ER115">
         <v>77.61</v>
       </c>
+      <c r="ES115">
+        <v>77.62</v>
+      </c>
     </row>
-    <row r="116" spans="1:148">
+    <row r="116" spans="1:149">
       <c r="A116" s="1">
         <v>35977</v>
       </c>
@@ -49647,8 +49992,11 @@
       <c r="ER116">
         <v>77.97</v>
       </c>
+      <c r="ES116">
+        <v>78</v>
+      </c>
     </row>
-    <row r="117" spans="1:148">
+    <row r="117" spans="1:149">
       <c r="A117" s="1">
         <v>36069</v>
       </c>
@@ -49970,8 +50318,11 @@
       <c r="ER117">
         <v>77.95</v>
       </c>
+      <c r="ES117">
+        <v>77.98</v>
+      </c>
     </row>
-    <row r="118" spans="1:148">
+    <row r="118" spans="1:149">
       <c r="A118" s="1">
         <v>36161</v>
       </c>
@@ -50290,8 +50641,11 @@
       <c r="ER118">
         <v>78.87</v>
       </c>
+      <c r="ES118">
+        <v>78.88</v>
+      </c>
     </row>
-    <row r="119" spans="1:148">
+    <row r="119" spans="1:149">
       <c r="A119" s="1">
         <v>36251</v>
       </c>
@@ -50607,8 +50961,11 @@
       <c r="ER119">
         <v>78.77</v>
       </c>
+      <c r="ES119">
+        <v>78.78</v>
+      </c>
     </row>
-    <row r="120" spans="1:148">
+    <row r="120" spans="1:149">
       <c r="A120" s="1">
         <v>36342</v>
       </c>
@@ -50921,8 +51278,11 @@
       <c r="ER120">
         <v>79.83</v>
       </c>
+      <c r="ES120">
+        <v>79.86</v>
+      </c>
     </row>
-    <row r="121" spans="1:148">
+    <row r="121" spans="1:149">
       <c r="A121" s="1">
         <v>36434</v>
       </c>
@@ -51232,8 +51592,11 @@
       <c r="ER121">
         <v>80.20999999999999</v>
       </c>
+      <c r="ES121">
+        <v>80.23999999999999</v>
+      </c>
     </row>
-    <row r="122" spans="1:148">
+    <row r="122" spans="1:149">
       <c r="A122" s="1">
         <v>36526</v>
       </c>
@@ -51540,8 +51903,11 @@
       <c r="ER122">
         <v>81.48</v>
       </c>
+      <c r="ES122">
+        <v>81.48</v>
+      </c>
     </row>
-    <row r="123" spans="1:148">
+    <row r="123" spans="1:149">
       <c r="A123" s="1">
         <v>36617</v>
       </c>
@@ -51845,8 +52211,11 @@
       <c r="ER123">
         <v>82.11</v>
       </c>
+      <c r="ES123">
+        <v>82.13</v>
+      </c>
     </row>
-    <row r="124" spans="1:148">
+    <row r="124" spans="1:149">
       <c r="A124" s="1">
         <v>36708</v>
       </c>
@@ -52147,8 +52516,11 @@
       <c r="ER124">
         <v>82.16</v>
       </c>
+      <c r="ES124">
+        <v>82.19</v>
+      </c>
     </row>
-    <row r="125" spans="1:148">
+    <row r="125" spans="1:149">
       <c r="A125" s="1">
         <v>36800</v>
       </c>
@@ -52446,8 +52818,11 @@
       <c r="ER125">
         <v>81.81</v>
       </c>
+      <c r="ES125">
+        <v>81.84</v>
+      </c>
     </row>
-    <row r="126" spans="1:148">
+    <row r="126" spans="1:149">
       <c r="A126" s="1">
         <v>36892</v>
       </c>
@@ -52742,8 +53117,11 @@
       <c r="ER126">
         <v>83.56999999999999</v>
       </c>
+      <c r="ES126">
+        <v>83.58</v>
+      </c>
     </row>
-    <row r="127" spans="1:148">
+    <row r="127" spans="1:149">
       <c r="A127" s="1">
         <v>36982</v>
       </c>
@@ -53035,8 +53413,11 @@
       <c r="ER127">
         <v>83.33</v>
       </c>
+      <c r="ES127">
+        <v>83.37</v>
+      </c>
     </row>
-    <row r="128" spans="1:148">
+    <row r="128" spans="1:149">
       <c r="A128" s="1">
         <v>37073</v>
       </c>
@@ -53325,8 +53706,11 @@
       <c r="ER128">
         <v>83.31999999999999</v>
       </c>
+      <c r="ES128">
+        <v>83.37</v>
+      </c>
     </row>
-    <row r="129" spans="1:148">
+    <row r="129" spans="1:149">
       <c r="A129" s="1">
         <v>37165</v>
       </c>
@@ -53612,8 +53996,11 @@
       <c r="ER129">
         <v>83.06999999999999</v>
       </c>
+      <c r="ES129">
+        <v>83.11</v>
+      </c>
     </row>
-    <row r="130" spans="1:148">
+    <row r="130" spans="1:149">
       <c r="A130" s="1">
         <v>37257</v>
       </c>
@@ -53896,8 +54283,11 @@
       <c r="ER130">
         <v>82.72</v>
       </c>
+      <c r="ES130">
+        <v>82.72</v>
+      </c>
     </row>
-    <row r="131" spans="1:148">
+    <row r="131" spans="1:149">
       <c r="A131" s="1">
         <v>37347</v>
       </c>
@@ -54177,8 +54567,11 @@
       <c r="ER131">
         <v>83.01000000000001</v>
       </c>
+      <c r="ES131">
+        <v>83.04000000000001</v>
+      </c>
     </row>
-    <row r="132" spans="1:148">
+    <row r="132" spans="1:149">
       <c r="A132" s="1">
         <v>37438</v>
       </c>
@@ -54455,8 +54848,11 @@
       <c r="ER132">
         <v>83.58</v>
       </c>
+      <c r="ES132">
+        <v>83.61</v>
+      </c>
     </row>
-    <row r="133" spans="1:148">
+    <row r="133" spans="1:149">
       <c r="A133" s="1">
         <v>37530</v>
       </c>
@@ -54730,8 +55126,11 @@
       <c r="ER133">
         <v>83.36</v>
       </c>
+      <c r="ES133">
+        <v>83.38</v>
+      </c>
     </row>
-    <row r="134" spans="1:148">
+    <row r="134" spans="1:149">
       <c r="A134" s="1">
         <v>37622</v>
       </c>
@@ -55002,8 +55401,11 @@
       <c r="ER134">
         <v>82.23999999999999</v>
       </c>
+      <c r="ES134">
+        <v>82.25</v>
+      </c>
     </row>
-    <row r="135" spans="1:148">
+    <row r="135" spans="1:149">
       <c r="A135" s="1">
         <v>37712</v>
       </c>
@@ -55271,8 +55673,11 @@
       <c r="ER135">
         <v>82.34</v>
       </c>
+      <c r="ES135">
+        <v>82.37</v>
+      </c>
     </row>
-    <row r="136" spans="1:148">
+    <row r="136" spans="1:149">
       <c r="A136" s="1">
         <v>37803</v>
       </c>
@@ -55537,8 +55942,11 @@
       <c r="ER136">
         <v>83.09</v>
       </c>
+      <c r="ES136">
+        <v>83.12</v>
+      </c>
     </row>
-    <row r="137" spans="1:148">
+    <row r="137" spans="1:149">
       <c r="A137" s="1">
         <v>37895</v>
       </c>
@@ -55800,8 +56208,11 @@
       <c r="ER137">
         <v>83.19</v>
       </c>
+      <c r="ES137">
+        <v>83.22</v>
+      </c>
     </row>
-    <row r="138" spans="1:148">
+    <row r="138" spans="1:149">
       <c r="A138" s="1">
         <v>37987</v>
       </c>
@@ -56060,8 +56471,11 @@
       <c r="ER138">
         <v>83.09</v>
       </c>
+      <c r="ES138">
+        <v>83.09</v>
+      </c>
     </row>
-    <row r="139" spans="1:148">
+    <row r="139" spans="1:149">
       <c r="A139" s="1">
         <v>38078</v>
       </c>
@@ -56317,8 +56731,11 @@
       <c r="ER139">
         <v>83.56</v>
       </c>
+      <c r="ES139">
+        <v>83.58</v>
+      </c>
     </row>
-    <row r="140" spans="1:148">
+    <row r="140" spans="1:149">
       <c r="A140" s="1">
         <v>38169</v>
       </c>
@@ -56571,8 +56988,11 @@
       <c r="ER140">
         <v>83.29000000000001</v>
       </c>
+      <c r="ES140">
+        <v>83.31</v>
+      </c>
     </row>
-    <row r="141" spans="1:148">
+    <row r="141" spans="1:149">
       <c r="A141" s="1">
         <v>38261</v>
       </c>
@@ -56822,8 +57242,11 @@
       <c r="ER141">
         <v>83.25</v>
       </c>
+      <c r="ES141">
+        <v>83.28</v>
+      </c>
     </row>
-    <row r="142" spans="1:148">
+    <row r="142" spans="1:149">
       <c r="A142" s="1">
         <v>38353</v>
       </c>
@@ -57070,8 +57493,11 @@
       <c r="ER142">
         <v>83.40000000000001</v>
       </c>
+      <c r="ES142">
+        <v>83.41</v>
+      </c>
     </row>
-    <row r="143" spans="1:148">
+    <row r="143" spans="1:149">
       <c r="A143" s="1">
         <v>38443</v>
       </c>
@@ -57315,8 +57741,11 @@
       <c r="ER143">
         <v>83.86</v>
       </c>
+      <c r="ES143">
+        <v>83.91</v>
+      </c>
     </row>
-    <row r="144" spans="1:148">
+    <row r="144" spans="1:149">
       <c r="A144" s="1">
         <v>38534</v>
       </c>
@@ -57557,8 +57986,11 @@
       <c r="ER144">
         <v>84.55</v>
       </c>
+      <c r="ES144">
+        <v>84.56999999999999</v>
+      </c>
     </row>
-    <row r="145" spans="1:148">
+    <row r="145" spans="1:149">
       <c r="A145" s="1">
         <v>38626</v>
       </c>
@@ -57796,8 +58228,11 @@
       <c r="ER145">
         <v>84.87</v>
       </c>
+      <c r="ES145">
+        <v>84.89</v>
+      </c>
     </row>
-    <row r="146" spans="1:148">
+    <row r="146" spans="1:149">
       <c r="A146" s="1">
         <v>38718</v>
       </c>
@@ -58032,8 +58467,11 @@
       <c r="ER146">
         <v>85.81999999999999</v>
       </c>
+      <c r="ES146">
+        <v>85.84</v>
+      </c>
     </row>
-    <row r="147" spans="1:148">
+    <row r="147" spans="1:149">
       <c r="A147" s="1">
         <v>38808</v>
       </c>
@@ -58265,8 +58703,11 @@
       <c r="ER147">
         <v>87.28</v>
       </c>
+      <c r="ES147">
+        <v>87.31</v>
+      </c>
     </row>
-    <row r="148" spans="1:148">
+    <row r="148" spans="1:149">
       <c r="A148" s="1">
         <v>38899</v>
       </c>
@@ -58495,8 +58936,11 @@
       <c r="ER148">
         <v>87.95999999999999</v>
       </c>
+      <c r="ES148">
+        <v>87.97</v>
+      </c>
     </row>
-    <row r="149" spans="1:148">
+    <row r="149" spans="1:149">
       <c r="A149" s="1">
         <v>38991</v>
       </c>
@@ -58722,8 +59166,11 @@
       <c r="ER149">
         <v>89.23999999999999</v>
       </c>
+      <c r="ES149">
+        <v>89.26000000000001</v>
+      </c>
     </row>
-    <row r="150" spans="1:148">
+    <row r="150" spans="1:149">
       <c r="A150" s="1">
         <v>39083</v>
       </c>
@@ -58946,8 +59393,11 @@
       <c r="ER150">
         <v>89.36</v>
       </c>
+      <c r="ES150">
+        <v>89.38</v>
+      </c>
     </row>
-    <row r="151" spans="1:148">
+    <row r="151" spans="1:149">
       <c r="A151" s="1">
         <v>39173</v>
       </c>
@@ -59167,8 +59617,11 @@
       <c r="ER151">
         <v>89.95</v>
       </c>
+      <c r="ES151">
+        <v>89.97</v>
+      </c>
     </row>
-    <row r="152" spans="1:148">
+    <row r="152" spans="1:149">
       <c r="A152" s="1">
         <v>39264</v>
       </c>
@@ -59385,8 +59838,11 @@
       <c r="ER152">
         <v>90.40000000000001</v>
       </c>
+      <c r="ES152">
+        <v>90.43000000000001</v>
+      </c>
     </row>
-    <row r="153" spans="1:148">
+    <row r="153" spans="1:149">
       <c r="A153" s="1">
         <v>39356</v>
       </c>
@@ -59600,8 +60056,11 @@
       <c r="ER153">
         <v>91.06999999999999</v>
       </c>
+      <c r="ES153">
+        <v>91.09999999999999</v>
+      </c>
     </row>
-    <row r="154" spans="1:148">
+    <row r="154" spans="1:149">
       <c r="A154" s="1">
         <v>39448</v>
       </c>
@@ -59812,8 +60271,11 @@
       <c r="ER154">
         <v>91.62</v>
       </c>
+      <c r="ES154">
+        <v>91.63</v>
+      </c>
     </row>
-    <row r="155" spans="1:148">
+    <row r="155" spans="1:149">
       <c r="A155" s="1">
         <v>39539</v>
       </c>
@@ -60021,8 +60483,11 @@
       <c r="ER155">
         <v>91.29000000000001</v>
       </c>
+      <c r="ES155">
+        <v>91.3</v>
+      </c>
     </row>
-    <row r="156" spans="1:148">
+    <row r="156" spans="1:149">
       <c r="A156" s="1">
         <v>39630</v>
       </c>
@@ -60227,8 +60692,11 @@
       <c r="ER156">
         <v>90.79000000000001</v>
       </c>
+      <c r="ES156">
+        <v>90.8</v>
+      </c>
     </row>
-    <row r="157" spans="1:148">
+    <row r="157" spans="1:149">
       <c r="A157" s="1">
         <v>39722</v>
       </c>
@@ -60430,8 +60898,11 @@
       <c r="ER157">
         <v>89.39</v>
       </c>
+      <c r="ES157">
+        <v>89.39</v>
+      </c>
     </row>
-    <row r="158" spans="1:148">
+    <row r="158" spans="1:149">
       <c r="A158" s="1">
         <v>39814</v>
       </c>
@@ -60630,8 +61101,11 @@
       <c r="ER158">
         <v>85.19</v>
       </c>
+      <c r="ES158">
+        <v>85.2</v>
+      </c>
     </row>
-    <row r="159" spans="1:148">
+    <row r="159" spans="1:149">
       <c r="A159" s="1">
         <v>39904</v>
       </c>
@@ -60827,8 +61301,11 @@
       <c r="ER159">
         <v>85.42</v>
       </c>
+      <c r="ES159">
+        <v>85.41</v>
+      </c>
     </row>
-    <row r="160" spans="1:148">
+    <row r="160" spans="1:149">
       <c r="A160" s="1">
         <v>39995</v>
       </c>
@@ -61021,8 +61498,11 @@
       <c r="ER160">
         <v>85.93000000000001</v>
       </c>
+      <c r="ES160">
+        <v>85.94</v>
+      </c>
     </row>
-    <row r="161" spans="1:148">
+    <row r="161" spans="1:149">
       <c r="A161" s="1">
         <v>40087</v>
       </c>
@@ -61212,8 +61692,11 @@
       <c r="ER161">
         <v>86.59999999999999</v>
       </c>
+      <c r="ES161">
+        <v>86.59999999999999</v>
+      </c>
     </row>
-    <row r="162" spans="1:148">
+    <row r="162" spans="1:149">
       <c r="A162" s="1">
         <v>40179</v>
       </c>
@@ -61400,8 +61883,11 @@
       <c r="ER162">
         <v>87.22</v>
       </c>
+      <c r="ES162">
+        <v>87.23</v>
+      </c>
     </row>
-    <row r="163" spans="1:148">
+    <row r="163" spans="1:149">
       <c r="A163" s="1">
         <v>40269</v>
       </c>
@@ -61585,8 +62071,11 @@
       <c r="ER163">
         <v>89.12</v>
       </c>
+      <c r="ES163">
+        <v>89.12</v>
+      </c>
     </row>
-    <row r="164" spans="1:148">
+    <row r="164" spans="1:149">
       <c r="A164" s="1">
         <v>40360</v>
       </c>
@@ -61767,8 +62256,11 @@
       <c r="ER164">
         <v>89.98</v>
       </c>
+      <c r="ES164">
+        <v>89.98</v>
+      </c>
     </row>
-    <row r="165" spans="1:148">
+    <row r="165" spans="1:149">
       <c r="A165" s="1">
         <v>40452</v>
       </c>
@@ -61946,8 +62438,11 @@
       <c r="ER165">
         <v>90.56999999999999</v>
       </c>
+      <c r="ES165">
+        <v>90.56999999999999</v>
+      </c>
     </row>
-    <row r="166" spans="1:148">
+    <row r="166" spans="1:149">
       <c r="A166" s="1">
         <v>40544</v>
       </c>
@@ -62122,8 +62617,11 @@
       <c r="ER166">
         <v>92.20999999999999</v>
       </c>
+      <c r="ES166">
+        <v>92.20999999999999</v>
+      </c>
     </row>
-    <row r="167" spans="1:148">
+    <row r="167" spans="1:149">
       <c r="A167" s="1">
         <v>40634</v>
       </c>
@@ -62295,8 +62793,11 @@
       <c r="ER167">
         <v>92.45999999999999</v>
       </c>
+      <c r="ES167">
+        <v>92.45999999999999</v>
+      </c>
     </row>
-    <row r="168" spans="1:148">
+    <row r="168" spans="1:149">
       <c r="A168" s="1">
         <v>40725</v>
       </c>
@@ -62465,8 +62966,11 @@
       <c r="ER168">
         <v>92.95999999999999</v>
       </c>
+      <c r="ES168">
+        <v>92.95999999999999</v>
+      </c>
     </row>
-    <row r="169" spans="1:148">
+    <row r="169" spans="1:149">
       <c r="A169" s="1">
         <v>40817</v>
       </c>
@@ -62632,8 +63136,11 @@
       <c r="ER169">
         <v>92.95999999999999</v>
       </c>
+      <c r="ES169">
+        <v>92.95</v>
+      </c>
     </row>
-    <row r="170" spans="1:148">
+    <row r="170" spans="1:149">
       <c r="A170" s="1">
         <v>40909</v>
       </c>
@@ -62796,8 +63303,11 @@
       <c r="ER170">
         <v>93.16</v>
       </c>
+      <c r="ES170">
+        <v>93.15000000000001</v>
+      </c>
     </row>
-    <row r="171" spans="1:148">
+    <row r="171" spans="1:149">
       <c r="A171" s="1">
         <v>41000</v>
       </c>
@@ -62957,8 +63467,11 @@
       <c r="ER171">
         <v>93.25</v>
       </c>
+      <c r="ES171">
+        <v>93.25</v>
+      </c>
     </row>
-    <row r="172" spans="1:148">
+    <row r="172" spans="1:149">
       <c r="A172" s="1">
         <v>41091</v>
       </c>
@@ -63115,8 +63628,11 @@
       <c r="ER172">
         <v>93.45</v>
       </c>
+      <c r="ES172">
+        <v>93.44</v>
+      </c>
     </row>
-    <row r="173" spans="1:148">
+    <row r="173" spans="1:149">
       <c r="A173" s="1">
         <v>41183</v>
       </c>
@@ -63270,8 +63786,11 @@
       <c r="ER173">
         <v>93.14</v>
       </c>
+      <c r="ES173">
+        <v>93.16</v>
+      </c>
     </row>
-    <row r="174" spans="1:148">
+    <row r="174" spans="1:149">
       <c r="A174" s="1">
         <v>41275</v>
       </c>
@@ -63422,8 +63941,11 @@
       <c r="ER174">
         <v>92.62</v>
       </c>
+      <c r="ES174">
+        <v>92.64</v>
+      </c>
     </row>
-    <row r="175" spans="1:148">
+    <row r="175" spans="1:149">
       <c r="A175" s="1">
         <v>41365</v>
       </c>
@@ -63571,8 +64093,11 @@
       <c r="ER175">
         <v>93.73999999999999</v>
       </c>
+      <c r="ES175">
+        <v>93.72</v>
+      </c>
     </row>
-    <row r="176" spans="1:148">
+    <row r="176" spans="1:149">
       <c r="A176" s="1">
         <v>41456</v>
       </c>
@@ -63717,8 +64242,11 @@
       <c r="ER176">
         <v>94.20999999999999</v>
       </c>
+      <c r="ES176">
+        <v>94.2</v>
+      </c>
     </row>
-    <row r="177" spans="1:148">
+    <row r="177" spans="1:149">
       <c r="A177" s="1">
         <v>41548</v>
       </c>
@@ -63860,8 +64388,11 @@
       <c r="ER177">
         <v>94.31999999999999</v>
       </c>
+      <c r="ES177">
+        <v>94.34</v>
+      </c>
     </row>
-    <row r="178" spans="1:148">
+    <row r="178" spans="1:149">
       <c r="A178" s="1">
         <v>41640</v>
       </c>
@@ -64000,8 +64531,11 @@
       <c r="ER178">
         <v>95.31</v>
       </c>
+      <c r="ES178">
+        <v>95.33</v>
+      </c>
     </row>
-    <row r="179" spans="1:148">
+    <row r="179" spans="1:149">
       <c r="A179" s="1">
         <v>41730</v>
       </c>
@@ -64137,8 +64671,11 @@
       <c r="ER179">
         <v>95.34</v>
       </c>
+      <c r="ES179">
+        <v>95.31</v>
+      </c>
     </row>
-    <row r="180" spans="1:148">
+    <row r="180" spans="1:149">
       <c r="A180" s="1">
         <v>41821</v>
       </c>
@@ -64271,8 +64808,11 @@
       <c r="ER180">
         <v>95.83</v>
       </c>
+      <c r="ES180">
+        <v>95.84</v>
+      </c>
     </row>
-    <row r="181" spans="1:148">
+    <row r="181" spans="1:149">
       <c r="A181" s="1">
         <v>41913</v>
       </c>
@@ -64402,8 +64942,11 @@
       <c r="ER181">
         <v>96.54000000000001</v>
       </c>
+      <c r="ES181">
+        <v>96.56999999999999</v>
+      </c>
     </row>
-    <row r="182" spans="1:148">
+    <row r="182" spans="1:149">
       <c r="A182" s="1">
         <v>42005</v>
       </c>
@@ -64530,8 +65073,11 @@
       <c r="ER182">
         <v>96.31999999999999</v>
       </c>
+      <c r="ES182">
+        <v>96.36</v>
+      </c>
     </row>
-    <row r="183" spans="1:148">
+    <row r="183" spans="1:149">
       <c r="A183" s="1">
         <v>42095</v>
       </c>
@@ -64655,8 +65201,11 @@
       <c r="ER183">
         <v>96.91</v>
       </c>
+      <c r="ES183">
+        <v>96.86</v>
+      </c>
     </row>
-    <row r="184" spans="1:148">
+    <row r="184" spans="1:149">
       <c r="A184" s="1">
         <v>42186</v>
       </c>
@@ -64777,8 +65326,11 @@
       <c r="ER184">
         <v>97.36</v>
       </c>
+      <c r="ES184">
+        <v>97.38</v>
+      </c>
     </row>
-    <row r="185" spans="1:148">
+    <row r="185" spans="1:149">
       <c r="A185" s="1">
         <v>42278</v>
       </c>
@@ -64896,8 +65448,11 @@
       <c r="ER185">
         <v>97.81</v>
       </c>
+      <c r="ES185">
+        <v>97.88</v>
+      </c>
     </row>
-    <row r="186" spans="1:148">
+    <row r="186" spans="1:149">
       <c r="A186" s="1">
         <v>42370</v>
       </c>
@@ -65012,8 +65567,11 @@
       <c r="ER186">
         <v>98.76000000000001</v>
       </c>
+      <c r="ES186">
+        <v>98.73999999999999</v>
+      </c>
     </row>
-    <row r="187" spans="1:148">
+    <row r="187" spans="1:149">
       <c r="A187" s="1">
         <v>42461</v>
       </c>
@@ -65125,8 +65683,11 @@
       <c r="ER187">
         <v>99.08</v>
       </c>
+      <c r="ES187">
+        <v>98.95999999999999</v>
+      </c>
     </row>
-    <row r="188" spans="1:148">
+    <row r="188" spans="1:149">
       <c r="A188" s="1">
         <v>42552</v>
       </c>
@@ -65235,8 +65796,11 @@
       <c r="ER188">
         <v>99.38</v>
       </c>
+      <c r="ES188">
+        <v>99.31</v>
+      </c>
     </row>
-    <row r="189" spans="1:148">
+    <row r="189" spans="1:149">
       <c r="A189" s="1">
         <v>42644</v>
       </c>
@@ -65342,8 +65906,11 @@
       <c r="ER189">
         <v>99.78</v>
       </c>
+      <c r="ES189">
+        <v>99.77</v>
+      </c>
     </row>
-    <row r="190" spans="1:148">
+    <row r="190" spans="1:149">
       <c r="A190" s="1">
         <v>42736</v>
       </c>
@@ -65446,8 +66013,11 @@
       <c r="ER190">
         <v>100.97</v>
       </c>
+      <c r="ES190">
+        <v>101.06</v>
+      </c>
     </row>
-    <row r="191" spans="1:148">
+    <row r="191" spans="1:149">
       <c r="A191" s="1">
         <v>42826</v>
       </c>
@@ -65547,8 +66117,11 @@
       <c r="ER191">
         <v>101.85</v>
       </c>
+      <c r="ES191">
+        <v>101.78</v>
+      </c>
     </row>
-    <row r="192" spans="1:148">
+    <row r="192" spans="1:149">
       <c r="A192" s="1">
         <v>42917</v>
       </c>
@@ -65645,8 +66218,11 @@
       <c r="ER192">
         <v>102.56</v>
       </c>
+      <c r="ES192">
+        <v>102.59</v>
+      </c>
     </row>
-    <row r="193" spans="1:148">
+    <row r="193" spans="1:149">
       <c r="A193" s="1">
         <v>43009</v>
       </c>
@@ -65740,8 +66316,11 @@
       <c r="ER193">
         <v>103.54</v>
       </c>
+      <c r="ES193">
+        <v>103.63</v>
+      </c>
     </row>
-    <row r="194" spans="1:148">
+    <row r="194" spans="1:149">
       <c r="A194" s="1">
         <v>43101</v>
       </c>
@@ -65832,8 +66411,11 @@
       <c r="ER194">
         <v>103.04</v>
       </c>
+      <c r="ES194">
+        <v>103.06</v>
+      </c>
     </row>
-    <row r="195" spans="1:148">
+    <row r="195" spans="1:149">
       <c r="A195" s="1">
         <v>43191</v>
       </c>
@@ -65921,8 +66503,11 @@
       <c r="ER195">
         <v>103.79</v>
       </c>
+      <c r="ES195">
+        <v>103.87</v>
+      </c>
     </row>
-    <row r="196" spans="1:148">
+    <row r="196" spans="1:149">
       <c r="A196" s="1">
         <v>43282</v>
       </c>
@@ -66007,8 +66592,11 @@
       <c r="ER196">
         <v>103.04</v>
       </c>
+      <c r="ES196">
+        <v>103.19</v>
+      </c>
     </row>
-    <row r="197" spans="1:148">
+    <row r="197" spans="1:149">
       <c r="A197" s="1">
         <v>43374</v>
       </c>
@@ -66090,8 +66678,11 @@
       <c r="ER197">
         <v>103.69</v>
       </c>
+      <c r="ES197">
+        <v>103.65</v>
+      </c>
     </row>
-    <row r="198" spans="1:148">
+    <row r="198" spans="1:149">
       <c r="A198" s="1">
         <v>43466</v>
       </c>
@@ -66170,8 +66761,11 @@
       <c r="ER198">
         <v>104.27</v>
       </c>
+      <c r="ES198">
+        <v>104.33</v>
+      </c>
     </row>
-    <row r="199" spans="1:148">
+    <row r="199" spans="1:149">
       <c r="A199" s="1">
         <v>43556</v>
       </c>
@@ -66247,8 +66841,11 @@
       <c r="ER199">
         <v>104.34</v>
       </c>
+      <c r="ES199">
+        <v>104.39</v>
+      </c>
     </row>
-    <row r="200" spans="1:148">
+    <row r="200" spans="1:149">
       <c r="A200" s="1">
         <v>43647</v>
       </c>
@@ -66321,8 +66918,11 @@
       <c r="ER200">
         <v>104.62</v>
       </c>
+      <c r="ES200">
+        <v>104.79</v>
+      </c>
     </row>
-    <row r="201" spans="1:148">
+    <row r="201" spans="1:149">
       <c r="A201" s="1">
         <v>43739</v>
       </c>
@@ -66392,8 +66992,11 @@
       <c r="ER201">
         <v>104.58</v>
       </c>
+      <c r="ES201">
+        <v>104.44</v>
+      </c>
     </row>
-    <row r="202" spans="1:148">
+    <row r="202" spans="1:149">
       <c r="A202" s="1">
         <v>43831</v>
       </c>
@@ -66460,8 +67063,11 @@
       <c r="ER202">
         <v>102.28</v>
       </c>
+      <c r="ES202">
+        <v>102.32</v>
+      </c>
     </row>
-    <row r="203" spans="1:148">
+    <row r="203" spans="1:149">
       <c r="A203" s="1">
         <v>43922</v>
       </c>
@@ -66525,8 +67131,11 @@
       <c r="ER203">
         <v>93.18000000000001</v>
       </c>
+      <c r="ES203">
+        <v>93.23999999999999</v>
+      </c>
     </row>
-    <row r="204" spans="1:148">
+    <row r="204" spans="1:149">
       <c r="A204" s="1">
         <v>44013</v>
       </c>
@@ -66587,8 +67196,11 @@
       <c r="ER204">
         <v>101.29</v>
       </c>
+      <c r="ES204">
+        <v>101.33</v>
+      </c>
     </row>
-    <row r="205" spans="1:148">
+    <row r="205" spans="1:149">
       <c r="A205" s="1">
         <v>44105</v>
       </c>
@@ -66646,8 +67258,11 @@
       <c r="ER205">
         <v>102.44</v>
       </c>
+      <c r="ES205">
+        <v>102.31</v>
+      </c>
     </row>
-    <row r="206" spans="1:148">
+    <row r="206" spans="1:149">
       <c r="A206" s="1">
         <v>44197</v>
       </c>
@@ -66702,8 +67317,11 @@
       <c r="ER206">
         <v>101.3</v>
       </c>
+      <c r="ES206">
+        <v>101.68</v>
+      </c>
     </row>
-    <row r="207" spans="1:148">
+    <row r="207" spans="1:149">
       <c r="A207" s="1">
         <v>44287</v>
       </c>
@@ -66755,8 +67373,11 @@
       <c r="ER207">
         <v>103.88</v>
       </c>
+      <c r="ES207">
+        <v>104.07</v>
+      </c>
     </row>
-    <row r="208" spans="1:148">
+    <row r="208" spans="1:149">
       <c r="A208" s="1">
         <v>44378</v>
       </c>
@@ -66805,8 +67426,11 @@
       <c r="ER208">
         <v>103.92</v>
       </c>
+      <c r="ES208">
+        <v>104.16</v>
+      </c>
     </row>
-    <row r="209" spans="1:148">
+    <row r="209" spans="1:149">
       <c r="A209" s="1">
         <v>44470</v>
       </c>
@@ -66852,8 +67476,11 @@
       <c r="ER209">
         <v>104.56</v>
       </c>
+      <c r="ES209">
+        <v>104.72</v>
+      </c>
     </row>
-    <row r="210" spans="1:148">
+    <row r="210" spans="1:149">
       <c r="A210" s="1">
         <v>44562</v>
       </c>
@@ -66896,8 +67523,11 @@
       <c r="ER210">
         <v>104.75</v>
       </c>
+      <c r="ES210">
+        <v>105.43</v>
+      </c>
     </row>
-    <row r="211" spans="1:148">
+    <row r="211" spans="1:149">
       <c r="A211" s="1">
         <v>44652</v>
       </c>
@@ -66937,8 +67567,11 @@
       <c r="ER211">
         <v>104.73</v>
       </c>
+      <c r="ES211">
+        <v>105.59</v>
+      </c>
     </row>
-    <row r="212" spans="1:148">
+    <row r="212" spans="1:149">
       <c r="A212" s="1">
         <v>44743</v>
       </c>
@@ -66975,8 +67608,11 @@
       <c r="ER212">
         <v>105.35</v>
       </c>
+      <c r="ES212">
+        <v>105.9</v>
+      </c>
     </row>
-    <row r="213" spans="1:148">
+    <row r="213" spans="1:149">
       <c r="A213" s="1">
         <v>44835</v>
       </c>
@@ -67010,8 +67646,11 @@
       <c r="ER213">
         <v>104.81</v>
       </c>
+      <c r="ES213">
+        <v>105.53</v>
+      </c>
     </row>
-    <row r="214" spans="1:148">
+    <row r="214" spans="1:149">
       <c r="A214" s="1">
         <v>44927</v>
       </c>
@@ -67042,8 +67681,11 @@
       <c r="ER214">
         <v>104.96</v>
       </c>
+      <c r="ES214">
+        <v>105.03</v>
+      </c>
     </row>
-    <row r="215" spans="1:148">
+    <row r="215" spans="1:149">
       <c r="A215" s="1">
         <v>45017</v>
       </c>
@@ -67071,8 +67713,11 @@
       <c r="ER215">
         <v>104.8</v>
       </c>
+      <c r="ES215">
+        <v>104.95</v>
+      </c>
     </row>
-    <row r="216" spans="1:148">
+    <row r="216" spans="1:149">
       <c r="A216" s="1">
         <v>45108</v>
       </c>
@@ -67097,8 +67742,11 @@
       <c r="ER216">
         <v>105</v>
       </c>
+      <c r="ES216">
+        <v>104.95</v>
+      </c>
     </row>
-    <row r="217" spans="1:148">
+    <row r="217" spans="1:149">
       <c r="A217" s="1">
         <v>45200</v>
       </c>
@@ -67120,8 +67768,11 @@
       <c r="ER217">
         <v>104.61</v>
       </c>
+      <c r="ES217">
+        <v>104.66</v>
+      </c>
     </row>
-    <row r="218" spans="1:148">
+    <row r="218" spans="1:149">
       <c r="A218" s="1">
         <v>45292</v>
       </c>
@@ -67140,8 +67791,11 @@
       <c r="ER218">
         <v>104.86</v>
       </c>
+      <c r="ES218">
+        <v>104.55</v>
+      </c>
     </row>
-    <row r="219" spans="1:148">
+    <row r="219" spans="1:149">
       <c r="A219" s="1">
         <v>45383</v>
       </c>
@@ -67157,8 +67811,11 @@
       <c r="ER219">
         <v>104.55</v>
       </c>
+      <c r="ES219">
+        <v>104.28</v>
+      </c>
     </row>
-    <row r="220" spans="1:148">
+    <row r="220" spans="1:149">
       <c r="A220" s="1">
         <v>45474</v>
       </c>
@@ -67171,8 +67828,11 @@
       <c r="ER220">
         <v>104.66</v>
       </c>
+      <c r="ES220">
+        <v>104.3</v>
+      </c>
     </row>
-    <row r="221" spans="1:148">
+    <row r="221" spans="1:149">
       <c r="A221" s="1">
         <v>45566</v>
       </c>
@@ -67182,13 +67842,27 @@
       <c r="ER221">
         <v>104.45</v>
       </c>
+      <c r="ES221">
+        <v>104.49</v>
+      </c>
     </row>
-    <row r="222" spans="1:148">
+    <row r="222" spans="1:149">
       <c r="A222" s="1">
         <v>45658</v>
       </c>
       <c r="ER222">
         <v>104.88</v>
+      </c>
+      <c r="ES222">
+        <v>104.81</v>
+      </c>
+    </row>
+    <row r="223" spans="1:149">
+      <c r="A223" s="1">
+        <v>45748</v>
+      </c>
+      <c r="ES223">
+        <v>104.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>